<commit_message>
Added log4j - working
</commit_message>
<xml_diff>
--- a/PageObjectModel/out/production/PageObjectModel/TestData/TestData.xlsx
+++ b/PageObjectModel/out/production/PageObjectModel/TestData/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Test Case Name</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Pass1</t>
   </si>
 </sst>
 </file>
@@ -279,7 +282,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>